<commit_message>
Move Chq Forms Code to cash account details
</commit_message>
<xml_diff>
--- a/Scripts/COH_Remittance.xlsx
+++ b/Scripts/COH_Remittance.xlsx
@@ -180,12 +180,12 @@
     <row r="2">
       <c r="a2" s="3" t="inlineStr">
         <is>
-          <t>DBTRACCTID</t>
+          <t>CHQFRMSCD</t>
         </is>
       </c>
       <c r="b2" s="3" t="inlineStr">
         <is>
-          <t>Debtor Account ID</t>
+          <t>Check Form Code</t>
         </is>
       </c>
       <c r="c2" s="3" t="inlineStr">
@@ -194,24 +194,24 @@
         </is>
       </c>
       <c r="d2" s="3" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="e2" s="3"/>
       <c r="f2" s="3" t="inlineStr">
         <is>
-          <t>^.{1,34}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="a3" s="3" t="inlineStr">
         <is>
-          <t>DBTRBLDGNB</t>
+          <t>DBTRACCTID</t>
         </is>
       </c>
       <c r="b3" s="3" t="inlineStr">
         <is>
-          <t>Debtor Building Number</t>
+          <t>Debtor Account ID</t>
         </is>
       </c>
       <c r="c3" s="3" t="inlineStr">
@@ -220,24 +220,24 @@
         </is>
       </c>
       <c r="d3" s="3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="e3" s="3"/>
       <c r="f3" s="3" t="inlineStr">
         <is>
-          <t>^.{1,16}$</t>
+          <t>^.{1,34}$</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="a4" s="3" t="inlineStr">
         <is>
-          <t>DBTRCNTRY</t>
+          <t>DBTRBLDGNB</t>
         </is>
       </c>
       <c r="b4" s="3" t="inlineStr">
         <is>
-          <t>Debtor Country</t>
+          <t>Debtor Building Number</t>
         </is>
       </c>
       <c r="c4" s="3" t="inlineStr">
@@ -246,24 +246,24 @@
         </is>
       </c>
       <c r="d4" s="3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="e4" s="3"/>
       <c r="f4" s="3" t="inlineStr">
         <is>
-          <t>^\w{2}$</t>
+          <t>^.{1,16}$</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="a5" s="3" t="inlineStr">
         <is>
-          <t>DBTRID</t>
+          <t>DBTRCNTRY</t>
         </is>
       </c>
       <c r="b5" s="3" t="inlineStr">
         <is>
-          <t>Debtor ID</t>
+          <t>Debtor Country</t>
         </is>
       </c>
       <c r="c5" s="3" t="inlineStr">
@@ -272,50 +272,50 @@
         </is>
       </c>
       <c r="d5" s="3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="e5" s="3"/>
       <c r="f5" s="3" t="inlineStr">
         <is>
-          <t>^.{1,35}$</t>
+          <t>^\w{2}$</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="a6" s="3" t="inlineStr">
         <is>
-          <t>DBTRNAME</t>
+          <t>DBTRID</t>
         </is>
       </c>
       <c r="b6" s="3" t="inlineStr">
         <is>
-          <t>Debtor Name</t>
+          <t>Debtor ID</t>
         </is>
       </c>
       <c r="c6" s="3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="d6" s="3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="e6" s="3"/>
       <c r="f6" s="3" t="inlineStr">
         <is>
-          <t>^.{1,140}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="a7" s="3" t="inlineStr">
         <is>
-          <t>DBTRSTATE</t>
+          <t>DBTRNAME</t>
         </is>
       </c>
       <c r="b7" s="3" t="inlineStr">
         <is>
-          <t>Debtor State/Province</t>
+          <t>Debtor Name</t>
         </is>
       </c>
       <c r="c7" s="3" t="inlineStr">
@@ -324,24 +324,24 @@
         </is>
       </c>
       <c r="d7" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="e7" s="3"/>
       <c r="f7" s="3" t="inlineStr">
         <is>
-          <t>^.{1,35}$</t>
+          <t>^.{1,140}$</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="a8" s="3" t="inlineStr">
         <is>
-          <t>DBTRSTNAME</t>
+          <t>DBTRSTATE</t>
         </is>
       </c>
       <c r="b8" s="3" t="inlineStr">
         <is>
-          <t>Debtor Street Name</t>
+          <t>Debtor State/Province</t>
         </is>
       </c>
       <c r="c8" s="3" t="inlineStr">
@@ -350,24 +350,24 @@
         </is>
       </c>
       <c r="d8" s="3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="e8" s="3"/>
       <c r="f8" s="3" t="inlineStr">
         <is>
-          <t>^.{1,70}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="a9" s="3" t="inlineStr">
         <is>
-          <t>DBTRTOWN</t>
+          <t>DBTRSTNAME</t>
         </is>
       </c>
       <c r="b9" s="3" t="inlineStr">
         <is>
-          <t>Debtor Town</t>
+          <t>Debtor Street Name</t>
         </is>
       </c>
       <c r="c9" s="3" t="inlineStr">
@@ -376,24 +376,24 @@
         </is>
       </c>
       <c r="d9" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="e9" s="3"/>
       <c r="f9" s="3" t="inlineStr">
         <is>
-          <t>^.{1,35}$</t>
+          <t>^.{1,70}$</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="a10" s="3" t="inlineStr">
         <is>
-          <t>DBTRZIP</t>
+          <t>DBTRTOWN</t>
         </is>
       </c>
       <c r="b10" s="3" t="inlineStr">
         <is>
-          <t>Debtor Zip/Postal Code</t>
+          <t>Debtor Town</t>
         </is>
       </c>
       <c r="c10" s="3" t="inlineStr">
@@ -402,24 +402,24 @@
         </is>
       </c>
       <c r="d10" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="e10" s="3"/>
       <c r="f10" s="3" t="inlineStr">
         <is>
-          <t>^.{1,16}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="a11" s="3" t="inlineStr">
         <is>
-          <t>FINBLDGNB</t>
+          <t>DBTRZIP</t>
         </is>
       </c>
       <c r="b11" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution Building Number</t>
+          <t>Debtor Zip/Postal Code</t>
         </is>
       </c>
       <c r="c11" s="3" t="inlineStr">
@@ -428,7 +428,7 @@
         </is>
       </c>
       <c r="d11" s="3" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="e11" s="3"/>
       <c r="f11" s="3" t="inlineStr">
@@ -440,12 +440,12 @@
     <row r="12">
       <c r="a12" s="3" t="inlineStr">
         <is>
-          <t>FINCNTRY</t>
+          <t>FINBLDGNB</t>
         </is>
       </c>
       <c r="b12" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution Country</t>
+          <t>Financial Institution Building Number</t>
         </is>
       </c>
       <c r="c12" s="3" t="inlineStr">
@@ -454,24 +454,24 @@
         </is>
       </c>
       <c r="d12" s="3" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="e12" s="3"/>
       <c r="f12" s="3" t="inlineStr">
         <is>
-          <t>^\w{2}$</t>
+          <t>^.{1,16}$</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="a13" s="3" t="inlineStr">
         <is>
-          <t>FININSTID</t>
+          <t>FINCNTRY</t>
         </is>
       </c>
       <c r="b13" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution ID</t>
+          <t>Financial Institution Country</t>
         </is>
       </c>
       <c r="c13" s="3" t="inlineStr">
@@ -480,24 +480,24 @@
         </is>
       </c>
       <c r="d13" s="3" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="e13" s="3"/>
       <c r="f13" s="3" t="inlineStr">
         <is>
-          <t>^.{1,35}$</t>
+          <t>^\w{2}$</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="a14" s="3" t="inlineStr">
         <is>
-          <t>FINSTATE</t>
+          <t>FININSTID</t>
         </is>
       </c>
       <c r="b14" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution State/Province</t>
+          <t>Financial Institution ID</t>
         </is>
       </c>
       <c r="c14" s="3" t="inlineStr">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="d14" s="3" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="e14" s="3"/>
       <c r="f14" s="3" t="inlineStr">
@@ -518,12 +518,12 @@
     <row r="15">
       <c r="a15" s="3" t="inlineStr">
         <is>
-          <t>FINSTNAME</t>
+          <t>FINSTATE</t>
         </is>
       </c>
       <c r="b15" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution Street Name</t>
+          <t>Financial Institution State/Province</t>
         </is>
       </c>
       <c r="c15" s="3" t="inlineStr">
@@ -532,24 +532,24 @@
         </is>
       </c>
       <c r="d15" s="3" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="e15" s="3"/>
       <c r="f15" s="3" t="inlineStr">
         <is>
-          <t>^.{1,70}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="a16" s="3" t="inlineStr">
         <is>
-          <t>FINTOWN</t>
+          <t>FINSTNAME</t>
         </is>
       </c>
       <c r="b16" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution Town</t>
+          <t>Financial Institution Street Name</t>
         </is>
       </c>
       <c r="c16" s="3" t="inlineStr">
@@ -558,24 +558,24 @@
         </is>
       </c>
       <c r="d16" s="3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="e16" s="3"/>
       <c r="f16" s="3" t="inlineStr">
         <is>
-          <t>^.{1,35}$</t>
+          <t>^.{1,70}$</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="a17" s="3" t="inlineStr">
         <is>
-          <t>FINZIP</t>
+          <t>FINTOWN</t>
         </is>
       </c>
       <c r="b17" s="3" t="inlineStr">
         <is>
-          <t>Financial Institution Zip/Postal Code</t>
+          <t>Financial Institution Town</t>
         </is>
       </c>
       <c r="c17" s="3" t="inlineStr">
@@ -584,24 +584,24 @@
         </is>
       </c>
       <c r="d17" s="3" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="e17" s="3"/>
       <c r="f17" s="3" t="inlineStr">
         <is>
-          <t>^.{1,16}$</t>
+          <t>^.{1,35}$</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="a18" s="3" t="inlineStr">
         <is>
-          <t>INITGPTYID</t>
+          <t>FINZIP</t>
         </is>
       </c>
       <c r="b18" s="3" t="inlineStr">
         <is>
-          <t>Initiating Party ID</t>
+          <t>Financial Institution Zip/Postal Code</t>
         </is>
       </c>
       <c r="c18" s="3" t="inlineStr">
@@ -610,10 +610,36 @@
         </is>
       </c>
       <c r="d18" s="3" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="e18" s="3"/>
       <c r="f18" s="3" t="inlineStr">
+        <is>
+          <t>^.{1,16}$</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="a19" s="3" t="inlineStr">
+        <is>
+          <t>INITGPTYID</t>
+        </is>
+      </c>
+      <c r="b19" s="3" t="inlineStr">
+        <is>
+          <t>Initiating Party ID</t>
+        </is>
+      </c>
+      <c r="c19" s="3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="d19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="e19" s="3"/>
+      <c r="f19" s="3" t="inlineStr">
         <is>
           <t>^.{1,35}$</t>
         </is>

</xml_diff>